<commit_message>
Added mocha, istanbul setup and 2 tests
</commit_message>
<xml_diff>
--- a/5_NodeJS/Demo-6July-Structure/map-dependencies.xlsx
+++ b/5_NodeJS/Demo-6July-Structure/map-dependencies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="20745" windowHeight="8895"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20745" windowHeight="8895"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3760,6 +3760,485 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3914775" y="4572000"/>
+          <a:ext cx="1219200" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>cookie-parser</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Rectangle 48"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3914775" y="4762500"/>
+          <a:ext cx="1219200" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>session</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="48" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3324225" y="3648076"/>
+          <a:ext cx="590550" cy="1019174"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="49" idx="1"/>
+          <a:endCxn id="5" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3305175" y="3619500"/>
+          <a:ext cx="609600" cy="1238250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Rectangle 56"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3914775" y="4953000"/>
+          <a:ext cx="1219200" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>connect-flash</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Rectangle 57"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3914775" y="5143500"/>
+          <a:ext cx="1219200" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>express-messages</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="57" idx="1"/>
+          <a:endCxn id="5" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3305175" y="3619500"/>
+          <a:ext cx="609600" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="58" idx="1"/>
+          <a:endCxn id="5" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3305175" y="3619500"/>
+          <a:ext cx="609600" cy="1619250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4029,7 +4508,7 @@
   <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>